<commit_message>
Inclusão módulo projeção baterias
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/custos.xlsx
+++ b/inst/dados_premissas/2023/custos.xlsx
@@ -1,18 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591A5113-AAF7-4268-B50D-7B1527C8A846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4364791C-4805-4787-81DF-9E79E8F7CF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="3135" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="custos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -123,2257 +120,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="custos"/>
-      <sheetName val="calculos"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B2">
-            <v>2013</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B3">
-            <v>2014</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B4">
-            <v>2015</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B5">
-            <v>2016</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B6">
-            <v>2017</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B7">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B8">
-            <v>2019</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B9">
-            <v>2020</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B10">
-            <v>2021</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B11">
-            <v>2022</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B12">
-            <v>2023</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B13">
-            <v>2024</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B14">
-            <v>2025</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B15">
-            <v>2026</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B16">
-            <v>2027</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B17">
-            <v>2028</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B18">
-            <v>2029</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B19">
-            <v>2030</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B20">
-            <v>2031</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B21">
-            <v>2032</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B22">
-            <v>2033</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B23">
-            <v>2034</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B24">
-            <v>2035</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B25">
-            <v>2036</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B26">
-            <v>2037</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B27">
-            <v>2038</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B28">
-            <v>2039</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B29">
-            <v>2040</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B30">
-            <v>2041</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B31">
-            <v>2042</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B32">
-            <v>2043</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B33">
-            <v>2044</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B34">
-            <v>2045</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B35">
-            <v>2046</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B36">
-            <v>2047</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B37">
-            <v>2048</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B38">
-            <v>2049</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B39">
-            <v>2050</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B50">
-            <v>2013</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B51">
-            <v>2014</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B52">
-            <v>2015</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B53">
-            <v>2016</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B54">
-            <v>2017</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B55">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B56">
-            <v>2019</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B57">
-            <v>2020</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B58">
-            <v>2021</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B59">
-            <v>2022</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B60">
-            <v>2023</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B61">
-            <v>2024</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B62">
-            <v>2025</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B63">
-            <v>2026</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B64">
-            <v>2027</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B65">
-            <v>2028</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B66">
-            <v>2029</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B67">
-            <v>2030</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B68">
-            <v>2031</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B69">
-            <v>2032</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B70">
-            <v>2033</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B71">
-            <v>2034</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B72">
-            <v>2035</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B73">
-            <v>2036</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B74">
-            <v>2037</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B75">
-            <v>2038</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B76">
-            <v>2039</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B77">
-            <v>2040</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B78">
-            <v>2041</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B79">
-            <v>2042</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B80">
-            <v>2043</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B81">
-            <v>2044</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B82">
-            <v>2045</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B83">
-            <v>2046</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B84">
-            <v>2047</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B85">
-            <v>2048</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B86">
-            <v>2049</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B87">
-            <v>2050</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B98">
-            <v>2013</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B99">
-            <v>2014</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B100">
-            <v>2015</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B101">
-            <v>2016</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B102">
-            <v>2017</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B103">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="A104" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B104">
-            <v>2019</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="A105" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B105">
-            <v>2020</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B106">
-            <v>2021</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="A107" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B107">
-            <v>2022</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="A108" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B108">
-            <v>2023</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="A109" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B109">
-            <v>2024</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B110">
-            <v>2025</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="A111" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B111">
-            <v>2026</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B112">
-            <v>2027</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="A113" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B113">
-            <v>2028</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="A114" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B114">
-            <v>2029</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B115">
-            <v>2030</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="A116" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B116">
-            <v>2031</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="A117" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B117">
-            <v>2032</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="A118" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B118">
-            <v>2033</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="A119" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B119">
-            <v>2034</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="A120" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B120">
-            <v>2035</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="A121" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B121">
-            <v>2036</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="A122" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B122">
-            <v>2037</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="A123" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B123">
-            <v>2038</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="A124" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B124">
-            <v>2039</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="A125" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B125">
-            <v>2040</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="A126" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B126">
-            <v>2041</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="A127" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B127">
-            <v>2042</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="A128" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B128">
-            <v>2043</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="A129" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B129">
-            <v>2044</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="A130" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B130">
-            <v>2045</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="A131" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B131">
-            <v>2046</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="A132" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B132">
-            <v>2047</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="A133" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B133">
-            <v>2048</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B134">
-            <v>2049</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="A135" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B135">
-            <v>2050</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="A146" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B146">
-            <v>2013</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="A147" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B147">
-            <v>2014</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="A148" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B148">
-            <v>2015</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="A149" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B149">
-            <v>2016</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="A150" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B150">
-            <v>2017</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="A151" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B151">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="A152" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B152">
-            <v>2019</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="A153" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B153">
-            <v>2020</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="A154" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B154">
-            <v>2021</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="A155" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B155">
-            <v>2022</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="A156" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B156">
-            <v>2023</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="A157" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B157">
-            <v>2024</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="A158" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B158">
-            <v>2025</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="A159" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B159">
-            <v>2026</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="A160" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B160">
-            <v>2027</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="A161" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B161">
-            <v>2028</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="A162" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B162">
-            <v>2029</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="A163" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B163">
-            <v>2030</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="A164" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B164">
-            <v>2031</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="A165" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B165">
-            <v>2032</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="A166" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B166">
-            <v>2033</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="A167" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B167">
-            <v>2034</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="A168" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B168">
-            <v>2035</v>
-          </cell>
-        </row>
-        <row r="169">
-          <cell r="A169" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B169">
-            <v>2036</v>
-          </cell>
-        </row>
-        <row r="170">
-          <cell r="A170" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B170">
-            <v>2037</v>
-          </cell>
-        </row>
-        <row r="171">
-          <cell r="A171" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B171">
-            <v>2038</v>
-          </cell>
-        </row>
-        <row r="172">
-          <cell r="A172" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B172">
-            <v>2039</v>
-          </cell>
-        </row>
-        <row r="173">
-          <cell r="A173" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B173">
-            <v>2040</v>
-          </cell>
-        </row>
-        <row r="174">
-          <cell r="A174" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B174">
-            <v>2041</v>
-          </cell>
-        </row>
-        <row r="175">
-          <cell r="A175" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B175">
-            <v>2042</v>
-          </cell>
-        </row>
-        <row r="176">
-          <cell r="A176" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B176">
-            <v>2043</v>
-          </cell>
-        </row>
-        <row r="177">
-          <cell r="A177" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B177">
-            <v>2044</v>
-          </cell>
-        </row>
-        <row r="178">
-          <cell r="A178" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B178">
-            <v>2045</v>
-          </cell>
-        </row>
-        <row r="179">
-          <cell r="A179" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B179">
-            <v>2046</v>
-          </cell>
-        </row>
-        <row r="180">
-          <cell r="A180" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B180">
-            <v>2047</v>
-          </cell>
-        </row>
-        <row r="181">
-          <cell r="A181" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B181">
-            <v>2048</v>
-          </cell>
-        </row>
-        <row r="182">
-          <cell r="A182" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B182">
-            <v>2049</v>
-          </cell>
-        </row>
-        <row r="183">
-          <cell r="A183" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B183">
-            <v>2050</v>
-          </cell>
-        </row>
-        <row r="194">
-          <cell r="A194" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B194">
-            <v>2013</v>
-          </cell>
-        </row>
-        <row r="195">
-          <cell r="A195" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B195">
-            <v>2014</v>
-          </cell>
-        </row>
-        <row r="196">
-          <cell r="A196" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B196">
-            <v>2015</v>
-          </cell>
-        </row>
-        <row r="197">
-          <cell r="A197" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B197">
-            <v>2016</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="A198" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B198">
-            <v>2017</v>
-          </cell>
-        </row>
-        <row r="199">
-          <cell r="A199" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B199">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="200">
-          <cell r="A200" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B200">
-            <v>2019</v>
-          </cell>
-        </row>
-        <row r="201">
-          <cell r="A201" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B201">
-            <v>2020</v>
-          </cell>
-        </row>
-        <row r="202">
-          <cell r="A202" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B202">
-            <v>2021</v>
-          </cell>
-        </row>
-        <row r="203">
-          <cell r="A203" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B203">
-            <v>2022</v>
-          </cell>
-        </row>
-        <row r="204">
-          <cell r="A204" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B204">
-            <v>2023</v>
-          </cell>
-        </row>
-        <row r="205">
-          <cell r="A205" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B205">
-            <v>2024</v>
-          </cell>
-        </row>
-        <row r="206">
-          <cell r="A206" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B206">
-            <v>2025</v>
-          </cell>
-        </row>
-        <row r="207">
-          <cell r="A207" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B207">
-            <v>2026</v>
-          </cell>
-        </row>
-        <row r="208">
-          <cell r="A208" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B208">
-            <v>2027</v>
-          </cell>
-        </row>
-        <row r="209">
-          <cell r="A209" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B209">
-            <v>2028</v>
-          </cell>
-        </row>
-        <row r="210">
-          <cell r="A210" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B210">
-            <v>2029</v>
-          </cell>
-        </row>
-        <row r="211">
-          <cell r="A211" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B211">
-            <v>2030</v>
-          </cell>
-        </row>
-        <row r="212">
-          <cell r="A212" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B212">
-            <v>2031</v>
-          </cell>
-        </row>
-        <row r="213">
-          <cell r="A213" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B213">
-            <v>2032</v>
-          </cell>
-        </row>
-        <row r="214">
-          <cell r="A214" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B214">
-            <v>2033</v>
-          </cell>
-        </row>
-        <row r="215">
-          <cell r="A215" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B215">
-            <v>2034</v>
-          </cell>
-        </row>
-        <row r="216">
-          <cell r="A216" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B216">
-            <v>2035</v>
-          </cell>
-        </row>
-        <row r="217">
-          <cell r="A217" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B217">
-            <v>2036</v>
-          </cell>
-        </row>
-        <row r="218">
-          <cell r="A218" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B218">
-            <v>2037</v>
-          </cell>
-        </row>
-        <row r="219">
-          <cell r="A219" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B219">
-            <v>2038</v>
-          </cell>
-        </row>
-        <row r="220">
-          <cell r="A220" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B220">
-            <v>2039</v>
-          </cell>
-        </row>
-        <row r="221">
-          <cell r="A221" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B221">
-            <v>2040</v>
-          </cell>
-        </row>
-        <row r="222">
-          <cell r="A222" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B222">
-            <v>2041</v>
-          </cell>
-        </row>
-        <row r="223">
-          <cell r="A223" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B223">
-            <v>2042</v>
-          </cell>
-        </row>
-        <row r="224">
-          <cell r="A224" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B224">
-            <v>2043</v>
-          </cell>
-        </row>
-        <row r="225">
-          <cell r="A225" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B225">
-            <v>2044</v>
-          </cell>
-        </row>
-        <row r="226">
-          <cell r="A226" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B226">
-            <v>2045</v>
-          </cell>
-        </row>
-        <row r="227">
-          <cell r="A227" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B227">
-            <v>2046</v>
-          </cell>
-        </row>
-        <row r="228">
-          <cell r="A228" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B228">
-            <v>2047</v>
-          </cell>
-        </row>
-        <row r="229">
-          <cell r="A229" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B229">
-            <v>2048</v>
-          </cell>
-        </row>
-        <row r="230">
-          <cell r="A230" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B230">
-            <v>2049</v>
-          </cell>
-        </row>
-        <row r="231">
-          <cell r="A231" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B231">
-            <v>2050</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="11">
-          <cell r="B11">
-            <v>2013</v>
-          </cell>
-          <cell r="C11">
-            <v>2014</v>
-          </cell>
-          <cell r="D11">
-            <v>2015</v>
-          </cell>
-          <cell r="E11">
-            <v>2016</v>
-          </cell>
-          <cell r="F11">
-            <v>2017</v>
-          </cell>
-          <cell r="G11">
-            <v>2018</v>
-          </cell>
-          <cell r="H11">
-            <v>2019</v>
-          </cell>
-          <cell r="I11">
-            <v>2020</v>
-          </cell>
-          <cell r="J11">
-            <v>2021</v>
-          </cell>
-          <cell r="K11">
-            <v>2022</v>
-          </cell>
-          <cell r="L11">
-            <v>2023</v>
-          </cell>
-          <cell r="M11">
-            <v>2024</v>
-          </cell>
-          <cell r="N11">
-            <v>2025</v>
-          </cell>
-          <cell r="O11">
-            <v>2026</v>
-          </cell>
-          <cell r="P11">
-            <v>2027</v>
-          </cell>
-          <cell r="Q11">
-            <v>2028</v>
-          </cell>
-          <cell r="R11">
-            <v>2029</v>
-          </cell>
-          <cell r="S11">
-            <v>2030</v>
-          </cell>
-          <cell r="T11">
-            <v>2031</v>
-          </cell>
-          <cell r="U11">
-            <v>2032</v>
-          </cell>
-          <cell r="V11">
-            <v>2033</v>
-          </cell>
-          <cell r="W11">
-            <v>2034</v>
-          </cell>
-          <cell r="X11">
-            <v>2035</v>
-          </cell>
-          <cell r="Y11">
-            <v>2036</v>
-          </cell>
-          <cell r="Z11">
-            <v>2037</v>
-          </cell>
-          <cell r="AA11">
-            <v>2038</v>
-          </cell>
-          <cell r="AB11">
-            <v>2039</v>
-          </cell>
-          <cell r="AC11">
-            <v>2040</v>
-          </cell>
-          <cell r="AD11">
-            <v>2041</v>
-          </cell>
-          <cell r="AE11">
-            <v>2042</v>
-          </cell>
-          <cell r="AF11">
-            <v>2043</v>
-          </cell>
-          <cell r="AG11">
-            <v>2044</v>
-          </cell>
-          <cell r="AH11">
-            <v>2045</v>
-          </cell>
-          <cell r="AI11">
-            <v>2046</v>
-          </cell>
-          <cell r="AJ11">
-            <v>2047</v>
-          </cell>
-          <cell r="AK11">
-            <v>2048</v>
-          </cell>
-          <cell r="AL11">
-            <v>2049</v>
-          </cell>
-          <cell r="AM11">
-            <v>2050</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>residencial</v>
-          </cell>
-          <cell r="B12">
-            <v>8.69</v>
-          </cell>
-          <cell r="C12">
-            <v>8.81</v>
-          </cell>
-          <cell r="D12">
-            <v>8.58</v>
-          </cell>
-          <cell r="E12">
-            <v>7.51</v>
-          </cell>
-          <cell r="F12">
-            <v>6.52</v>
-          </cell>
-          <cell r="G12">
-            <v>5.76</v>
-          </cell>
-          <cell r="H12">
-            <v>5</v>
-          </cell>
-          <cell r="I12">
-            <v>4.76</v>
-          </cell>
-          <cell r="J12">
-            <v>4.88</v>
-          </cell>
-          <cell r="K12">
-            <v>4.88</v>
-          </cell>
-          <cell r="L12">
-            <v>3.68</v>
-          </cell>
-          <cell r="M12">
-            <v>2.93</v>
-          </cell>
-          <cell r="N12">
-            <v>2.8456160000000001</v>
-          </cell>
-          <cell r="O12">
-            <v>2.7636622592000002</v>
-          </cell>
-          <cell r="P12">
-            <v>2.6840687861350401</v>
-          </cell>
-          <cell r="Q12">
-            <v>2.6067676050943507</v>
-          </cell>
-          <cell r="R12">
-            <v>2.5316926980676331</v>
-          </cell>
-          <cell r="S12">
-            <v>2.4587799483632851</v>
-          </cell>
-          <cell r="T12">
-            <v>2.4225562163949754</v>
-          </cell>
-          <cell r="U12">
-            <v>2.3868661469687673</v>
-          </cell>
-          <cell r="V12">
-            <v>2.3517018779541359</v>
-          </cell>
-          <cell r="W12">
-            <v>2.3170556630486145</v>
-          </cell>
-          <cell r="X12">
-            <v>2.2829198700713711</v>
-          </cell>
-          <cell r="Y12">
-            <v>2.2492869792819206</v>
-          </cell>
-          <cell r="Z12">
-            <v>2.2161495817236099</v>
-          </cell>
-          <cell r="AA12">
-            <v>2.1835003775915056</v>
-          </cell>
-          <cell r="AB12">
-            <v>2.1513321746243275</v>
-          </cell>
-          <cell r="AC12">
-            <v>2.119637886520072</v>
-          </cell>
-          <cell r="AD12">
-            <v>2.0915222007350893</v>
-          </cell>
-          <cell r="AE12">
-            <v>2.0637794521353618</v>
-          </cell>
-          <cell r="AF12">
-            <v>2.0364046939397511</v>
-          </cell>
-          <cell r="AG12">
-            <v>2.0093930449831112</v>
-          </cell>
-          <cell r="AH12">
-            <v>1.982739688845933</v>
-          </cell>
-          <cell r="AI12">
-            <v>1.9564398729955339</v>
-          </cell>
-          <cell r="AJ12">
-            <v>1.9304889079386385</v>
-          </cell>
-          <cell r="AK12">
-            <v>1.9048821663851994</v>
-          </cell>
-          <cell r="AL12">
-            <v>1.8796150824233102</v>
-          </cell>
-          <cell r="AM12">
-            <v>1.854683150705063</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>residencial_remoto</v>
-          </cell>
-          <cell r="B13">
-            <v>7.7303680981595102</v>
-          </cell>
-          <cell r="C13">
-            <v>7.8371165644171796</v>
-          </cell>
-          <cell r="D13">
-            <v>7.6325153374233139</v>
-          </cell>
-          <cell r="E13">
-            <v>6.6806748466257675</v>
-          </cell>
-          <cell r="F13">
-            <v>5.8</v>
-          </cell>
-          <cell r="G13">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="H13">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="I13">
-            <v>4.2699999999999996</v>
-          </cell>
-          <cell r="J13">
-            <v>4.38</v>
-          </cell>
-          <cell r="K13">
-            <v>4.3499999999999996</v>
-          </cell>
-          <cell r="L13">
-            <v>3.26</v>
-          </cell>
-          <cell r="M13">
-            <v>2.58</v>
-          </cell>
-          <cell r="N13">
-            <v>2.5056959999999999</v>
-          </cell>
-          <cell r="O13">
-            <v>2.4335319551999999</v>
-          </cell>
-          <cell r="P13">
-            <v>2.3634462348902399</v>
-          </cell>
-          <cell r="Q13">
-            <v>2.295378983325401</v>
-          </cell>
-          <cell r="R13">
-            <v>2.2292720686056295</v>
-          </cell>
-          <cell r="S13">
-            <v>2.1650690330297873</v>
-          </cell>
-          <cell r="T13">
-            <v>2.1331723680201495</v>
-          </cell>
-          <cell r="U13">
-            <v>2.1017456174673792</v>
-          </cell>
-          <cell r="V13">
-            <v>2.0707818584033011</v>
-          </cell>
-          <cell r="W13">
-            <v>2.0402742698516816</v>
-          </cell>
-          <cell r="X13">
-            <v>2.0102161313256444</v>
-          </cell>
-          <cell r="Y13">
-            <v>1.9806008213472202</v>
-          </cell>
-          <cell r="Z13">
-            <v>1.9514218159887076</v>
-          </cell>
-          <cell r="AA13">
-            <v>1.9226726874355238</v>
-          </cell>
-          <cell r="AB13">
-            <v>1.8943471025702272</v>
-          </cell>
-          <cell r="AC13">
-            <v>1.8664388215774017</v>
-          </cell>
-          <cell r="AD13">
-            <v>1.8416816648111027</v>
-          </cell>
-          <cell r="AE13">
-            <v>1.817252896419534</v>
-          </cell>
-          <cell r="AF13">
-            <v>1.7931481605339794</v>
-          </cell>
-          <cell r="AG13">
-            <v>1.7693631590636276</v>
-          </cell>
-          <cell r="AH13">
-            <v>1.745893650929184</v>
-          </cell>
-          <cell r="AI13">
-            <v>1.7227354513066484</v>
-          </cell>
-          <cell r="AJ13">
-            <v>1.6998844308811227</v>
-          </cell>
-          <cell r="AK13">
-            <v>1.6773365151105175</v>
-          </cell>
-          <cell r="AL13">
-            <v>1.6550876834990247</v>
-          </cell>
-          <cell r="AM13">
-            <v>1.6331339688802267</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>comercial_bt</v>
-          </cell>
-          <cell r="B14">
-            <v>6.97</v>
-          </cell>
-          <cell r="C14">
-            <v>7.85</v>
-          </cell>
-          <cell r="D14">
-            <v>7.57</v>
-          </cell>
-          <cell r="E14">
-            <v>6.73</v>
-          </cell>
-          <cell r="F14">
-            <v>5.59</v>
-          </cell>
-          <cell r="G14">
-            <v>5.01</v>
-          </cell>
-          <cell r="H14">
-            <v>4.2</v>
-          </cell>
-          <cell r="I14">
-            <v>4.1100000000000003</v>
-          </cell>
-          <cell r="J14">
-            <v>4.21</v>
-          </cell>
-          <cell r="K14">
-            <v>4.16</v>
-          </cell>
-          <cell r="L14">
-            <v>3.02</v>
-          </cell>
-          <cell r="M14">
-            <v>2.3199999999999998</v>
-          </cell>
-          <cell r="N14">
-            <v>2.2531839999999996</v>
-          </cell>
-          <cell r="O14">
-            <v>2.1882923007999997</v>
-          </cell>
-          <cell r="P14">
-            <v>2.1252694825369596</v>
-          </cell>
-          <cell r="Q14">
-            <v>2.0640617214398951</v>
-          </cell>
-          <cell r="R14">
-            <v>2.0046167438624258</v>
-          </cell>
-          <cell r="S14">
-            <v>1.946883781639188</v>
-          </cell>
-          <cell r="T14">
-            <v>1.9182015092274207</v>
-          </cell>
-          <cell r="U14">
-            <v>1.8899417955520614</v>
-          </cell>
-          <cell r="V14">
-            <v>1.8620984153083942</v>
-          </cell>
-          <cell r="W14">
-            <v>1.8346652349053876</v>
-          </cell>
-          <cell r="X14">
-            <v>1.8076362111145325</v>
-          </cell>
-          <cell r="Y14">
-            <v>1.7810053897385854</v>
-          </cell>
-          <cell r="Z14">
-            <v>1.754766904299923</v>
-          </cell>
-          <cell r="AA14">
-            <v>1.7289149747482229</v>
-          </cell>
-          <cell r="AB14">
-            <v>1.7034439061871809</v>
-          </cell>
-          <cell r="AC14">
-            <v>1.678348087619989</v>
-          </cell>
-          <cell r="AD14">
-            <v>1.6560858381247123</v>
-          </cell>
-          <cell r="AE14">
-            <v>1.6341188836020613</v>
-          </cell>
-          <cell r="AF14">
-            <v>1.6124433071468338</v>
-          </cell>
-          <cell r="AG14">
-            <v>1.591055243809153</v>
-          </cell>
-          <cell r="AH14">
-            <v>1.5699508799053121</v>
-          </cell>
-          <cell r="AI14">
-            <v>1.5491264523377606</v>
-          </cell>
-          <cell r="AJ14">
-            <v>1.5285782479241095</v>
-          </cell>
-          <cell r="AK14">
-            <v>1.5083026027350381</v>
-          </cell>
-          <cell r="AL14">
-            <v>1.4882959014409827</v>
-          </cell>
-          <cell r="AM14">
-            <v>1.4685545766674899</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>comercial_at</v>
-          </cell>
-          <cell r="B15">
-            <v>6.69</v>
-          </cell>
-          <cell r="C15">
-            <v>6.98</v>
-          </cell>
-          <cell r="D15">
-            <v>6.86</v>
-          </cell>
-          <cell r="E15">
-            <v>6.16</v>
-          </cell>
-          <cell r="F15">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="G15">
-            <v>4.2300000000000004</v>
-          </cell>
-          <cell r="H15">
-            <v>3.4</v>
-          </cell>
-          <cell r="I15">
-            <v>3.62</v>
-          </cell>
-          <cell r="J15">
-            <v>3.81</v>
-          </cell>
-          <cell r="K15">
-            <v>4</v>
-          </cell>
-          <cell r="L15">
-            <v>3.03</v>
-          </cell>
-          <cell r="M15">
-            <v>2.57</v>
-          </cell>
-          <cell r="N15">
-            <v>2.4959839999999995</v>
-          </cell>
-          <cell r="O15">
-            <v>2.4240996607999996</v>
-          </cell>
-          <cell r="P15">
-            <v>2.3542855905689595</v>
-          </cell>
-          <cell r="Q15">
-            <v>2.2864821655605732</v>
-          </cell>
-          <cell r="R15">
-            <v>2.2206314791924284</v>
-          </cell>
-          <cell r="S15">
-            <v>2.1566772925916862</v>
-          </cell>
-          <cell r="T15">
-            <v>2.1249042580665818</v>
-          </cell>
-          <cell r="U15">
-            <v>2.0935993166244811</v>
-          </cell>
-          <cell r="V15">
-            <v>2.0627555721304187</v>
-          </cell>
-          <cell r="W15">
-            <v>2.0323662300460534</v>
-          </cell>
-          <cell r="X15">
-            <v>2.0024245959329079</v>
-          </cell>
-          <cell r="Y15">
-            <v>1.9729240739776559</v>
-          </cell>
-          <cell r="Z15">
-            <v>1.9438581655391376</v>
-          </cell>
-          <cell r="AA15">
-            <v>1.9152204677167801</v>
-          </cell>
-          <cell r="AB15">
-            <v>1.8870046719401088</v>
-          </cell>
-          <cell r="AC15">
-            <v>1.8592045625790383</v>
-          </cell>
-          <cell r="AD15">
-            <v>1.8345433637847017</v>
-          </cell>
-          <cell r="AE15">
-            <v>1.8102092805419374</v>
-          </cell>
-          <cell r="AF15">
-            <v>1.7861979738652414</v>
-          </cell>
-          <cell r="AG15">
-            <v>1.7625051623230692</v>
-          </cell>
-          <cell r="AH15">
-            <v>1.7391266212744181</v>
-          </cell>
-          <cell r="AI15">
-            <v>1.7160581821155356</v>
-          </cell>
-          <cell r="AJ15">
-            <v>1.6932957315366204</v>
-          </cell>
-          <cell r="AK15">
-            <v>1.6708352107883819</v>
-          </cell>
-          <cell r="AL15">
-            <v>1.6486726149583291</v>
-          </cell>
-          <cell r="AM15">
-            <v>1.6268039922566582</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>comercial_at_remoto</v>
-          </cell>
-          <cell r="B16">
-            <v>6.8203246753246765</v>
-          </cell>
-          <cell r="C16">
-            <v>7.115974025974027</v>
-          </cell>
-          <cell r="D16">
-            <v>6.993636363636365</v>
-          </cell>
-          <cell r="E16">
-            <v>6.28</v>
-          </cell>
-          <cell r="F16">
-            <v>4.47</v>
-          </cell>
-          <cell r="G16">
-            <v>4.2300000000000004</v>
-          </cell>
-          <cell r="H16">
-            <v>3.5</v>
-          </cell>
-          <cell r="I16">
-            <v>3.85</v>
-          </cell>
-          <cell r="J16">
-            <v>4.08</v>
-          </cell>
-          <cell r="K16">
-            <v>4.45</v>
-          </cell>
-          <cell r="L16">
-            <v>3.64</v>
-          </cell>
-          <cell r="M16">
-            <v>3.13</v>
-          </cell>
-          <cell r="N16">
-            <v>3.0398559999999999</v>
-          </cell>
-          <cell r="O16">
-            <v>2.9523081471999997</v>
-          </cell>
-          <cell r="P16">
-            <v>2.8672816725606394</v>
-          </cell>
-          <cell r="Q16">
-            <v>2.784703960390893</v>
-          </cell>
-          <cell r="R16">
-            <v>2.704504486331635</v>
-          </cell>
-          <cell r="S16">
-            <v>2.6266147571252838</v>
-          </cell>
-          <cell r="T16">
-            <v>2.5879184154663046</v>
-          </cell>
-          <cell r="U16">
-            <v>2.5497921638267038</v>
-          </cell>
-          <cell r="V16">
-            <v>2.5122276034117563</v>
-          </cell>
-          <cell r="W16">
-            <v>2.4752164591611483</v>
-          </cell>
-          <cell r="X16">
-            <v>2.4387505779260725</v>
-          </cell>
-          <cell r="Y16">
-            <v>2.4028219266731781</v>
-          </cell>
-          <cell r="Z16">
-            <v>2.3674225907149826</v>
-          </cell>
-          <cell r="AA16">
-            <v>2.3325447719663526</v>
-          </cell>
-          <cell r="AB16">
-            <v>2.2981807872266709</v>
-          </cell>
-          <cell r="AC16">
-            <v>2.2643230664873126</v>
-          </cell>
-          <cell r="AD16">
-            <v>2.2342882212630819</v>
-          </cell>
-          <cell r="AE16">
-            <v>2.2046517696872638</v>
-          </cell>
-          <cell r="AF16">
-            <v>2.1754084273144785</v>
-          </cell>
-          <cell r="AG16">
-            <v>2.1465529797942455</v>
-          </cell>
-          <cell r="AH16">
-            <v>2.1180802819412188</v>
-          </cell>
-          <cell r="AI16">
-            <v>2.089985256817755</v>
-          </cell>
-          <cell r="AJ16">
-            <v>2.0622628948286481</v>
-          </cell>
-          <cell r="AK16">
-            <v>2.0349082528278752</v>
-          </cell>
-          <cell r="AL16">
-            <v>2.0079164532371885</v>
-          </cell>
-          <cell r="AM16">
-            <v>1.9812826831763986</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2641,9 +387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C241"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2670,7 +414,6 @@
         <v>2013</v>
       </c>
       <c r="C2" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A2,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B2,[1]calculos!$B$11:$AM$11,0))</f>
         <v>8.69</v>
       </c>
     </row>
@@ -2682,7 +425,6 @@
         <v>2014</v>
       </c>
       <c r="C3" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A3,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B3,[1]calculos!$B$11:$AM$11,0))</f>
         <v>8.81</v>
       </c>
     </row>
@@ -2694,7 +436,6 @@
         <v>2015</v>
       </c>
       <c r="C4" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A4,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B4,[1]calculos!$B$11:$AM$11,0))</f>
         <v>8.58</v>
       </c>
     </row>
@@ -2706,7 +447,6 @@
         <v>2016</v>
       </c>
       <c r="C5" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A5,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B5,[1]calculos!$B$11:$AM$11,0))</f>
         <v>7.51</v>
       </c>
     </row>
@@ -2718,7 +458,6 @@
         <v>2017</v>
       </c>
       <c r="C6" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A6,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B6,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.52</v>
       </c>
     </row>
@@ -2730,7 +469,6 @@
         <v>2018</v>
       </c>
       <c r="C7" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A7,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B7,[1]calculos!$B$11:$AM$11,0))</f>
         <v>5.76</v>
       </c>
     </row>
@@ -2742,7 +480,6 @@
         <v>2019</v>
       </c>
       <c r="C8" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A8,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B8,[1]calculos!$B$11:$AM$11,0))</f>
         <v>5</v>
       </c>
     </row>
@@ -2754,7 +491,6 @@
         <v>2020</v>
       </c>
       <c r="C9" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A9,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B9,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.76</v>
       </c>
     </row>
@@ -2766,7 +502,6 @@
         <v>2021</v>
       </c>
       <c r="C10" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A10,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B10,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.88</v>
       </c>
     </row>
@@ -2778,7 +513,6 @@
         <v>2022</v>
       </c>
       <c r="C11" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A11,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B11,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.88</v>
       </c>
     </row>
@@ -2790,7 +524,6 @@
         <v>2023</v>
       </c>
       <c r="C12" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A12,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B12,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.68</v>
       </c>
     </row>
@@ -2802,7 +535,6 @@
         <v>2024</v>
       </c>
       <c r="C13" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A13,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B13,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.93</v>
       </c>
     </row>
@@ -2814,7 +546,6 @@
         <v>2025</v>
       </c>
       <c r="C14" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A14,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B14,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.8456160000000001</v>
       </c>
     </row>
@@ -2826,7 +557,6 @@
         <v>2026</v>
       </c>
       <c r="C15" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A15,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B15,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.7636622592000002</v>
       </c>
     </row>
@@ -2838,7 +568,6 @@
         <v>2027</v>
       </c>
       <c r="C16" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A16,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B16,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.6840687861350401</v>
       </c>
     </row>
@@ -2850,7 +579,6 @@
         <v>2028</v>
       </c>
       <c r="C17" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A17,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B17,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.6067676050943507</v>
       </c>
     </row>
@@ -2862,7 +590,6 @@
         <v>2029</v>
       </c>
       <c r="C18" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A18,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B18,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.5316926980676331</v>
       </c>
     </row>
@@ -2874,7 +601,6 @@
         <v>2030</v>
       </c>
       <c r="C19" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A19,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B19,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4587799483632851</v>
       </c>
     </row>
@@ -2886,7 +612,6 @@
         <v>2031</v>
       </c>
       <c r="C20" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A20,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B20,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4225562163949754</v>
       </c>
     </row>
@@ -2898,7 +623,6 @@
         <v>2032</v>
       </c>
       <c r="C21" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A21,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B21,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3868661469687673</v>
       </c>
     </row>
@@ -2910,7 +634,6 @@
         <v>2033</v>
       </c>
       <c r="C22" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A22,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B22,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3517018779541359</v>
       </c>
     </row>
@@ -2922,7 +645,6 @@
         <v>2034</v>
       </c>
       <c r="C23" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A23,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B23,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3170556630486145</v>
       </c>
     </row>
@@ -2934,7 +656,6 @@
         <v>2035</v>
       </c>
       <c r="C24" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A24,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B24,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2829198700713711</v>
       </c>
     </row>
@@ -2946,7 +667,6 @@
         <v>2036</v>
       </c>
       <c r="C25" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A25,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B25,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2492869792819206</v>
       </c>
     </row>
@@ -2958,7 +678,6 @@
         <v>2037</v>
       </c>
       <c r="C26" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A26,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B26,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2161495817236099</v>
       </c>
     </row>
@@ -2970,7 +689,6 @@
         <v>2038</v>
       </c>
       <c r="C27" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A27,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B27,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1835003775915056</v>
       </c>
     </row>
@@ -2982,7 +700,6 @@
         <v>2039</v>
       </c>
       <c r="C28" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A28,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B28,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1513321746243275</v>
       </c>
     </row>
@@ -2994,7 +711,6 @@
         <v>2040</v>
       </c>
       <c r="C29" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A29,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B29,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.119637886520072</v>
       </c>
     </row>
@@ -3006,7 +722,6 @@
         <v>2041</v>
       </c>
       <c r="C30" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A30,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B30,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0915222007350893</v>
       </c>
     </row>
@@ -3018,7 +733,6 @@
         <v>2042</v>
       </c>
       <c r="C31" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A31,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B31,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0637794521353618</v>
       </c>
     </row>
@@ -3030,7 +744,6 @@
         <v>2043</v>
       </c>
       <c r="C32" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A32,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B32,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0364046939397511</v>
       </c>
     </row>
@@ -3042,7 +755,6 @@
         <v>2044</v>
       </c>
       <c r="C33" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A33,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B33,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0093930449831112</v>
       </c>
     </row>
@@ -3054,7 +766,6 @@
         <v>2045</v>
       </c>
       <c r="C34" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A34,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B34,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.982739688845933</v>
       </c>
     </row>
@@ -3066,7 +777,6 @@
         <v>2046</v>
       </c>
       <c r="C35" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A35,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B35,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9564398729955339</v>
       </c>
     </row>
@@ -3078,7 +788,6 @@
         <v>2047</v>
       </c>
       <c r="C36" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A36,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B36,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9304889079386385</v>
       </c>
     </row>
@@ -3090,7 +799,6 @@
         <v>2048</v>
       </c>
       <c r="C37" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A37,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B37,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9048821663851994</v>
       </c>
     </row>
@@ -3102,7 +810,6 @@
         <v>2049</v>
       </c>
       <c r="C38" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A38,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B38,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8796150824233102</v>
       </c>
     </row>
@@ -3114,7 +821,6 @@
         <v>2050</v>
       </c>
       <c r="C39" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A39,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B39,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.854683150705063</v>
       </c>
     </row>
@@ -3246,7 +952,6 @@
         <v>2013</v>
       </c>
       <c r="C50" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A50,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B50,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.97</v>
       </c>
     </row>
@@ -3258,7 +963,6 @@
         <v>2014</v>
       </c>
       <c r="C51" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A51,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B51,[1]calculos!$B$11:$AM$11,0))</f>
         <v>7.85</v>
       </c>
     </row>
@@ -3270,7 +974,6 @@
         <v>2015</v>
       </c>
       <c r="C52" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A52,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B52,[1]calculos!$B$11:$AM$11,0))</f>
         <v>7.57</v>
       </c>
     </row>
@@ -3282,7 +985,6 @@
         <v>2016</v>
       </c>
       <c r="C53" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A53,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B53,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.73</v>
       </c>
     </row>
@@ -3294,7 +996,6 @@
         <v>2017</v>
       </c>
       <c r="C54" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A54,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B54,[1]calculos!$B$11:$AM$11,0))</f>
         <v>5.59</v>
       </c>
     </row>
@@ -3306,7 +1007,6 @@
         <v>2018</v>
       </c>
       <c r="C55" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A55,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B55,[1]calculos!$B$11:$AM$11,0))</f>
         <v>5.01</v>
       </c>
     </row>
@@ -3318,7 +1018,6 @@
         <v>2019</v>
       </c>
       <c r="C56" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A56,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B56,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.2</v>
       </c>
     </row>
@@ -3330,7 +1029,6 @@
         <v>2020</v>
       </c>
       <c r="C57" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A57,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B57,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.1100000000000003</v>
       </c>
     </row>
@@ -3342,7 +1040,6 @@
         <v>2021</v>
       </c>
       <c r="C58" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A58,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B58,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.21</v>
       </c>
     </row>
@@ -3354,7 +1051,6 @@
         <v>2022</v>
       </c>
       <c r="C59" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A59,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B59,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.16</v>
       </c>
     </row>
@@ -3366,7 +1062,6 @@
         <v>2023</v>
       </c>
       <c r="C60" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A60,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B60,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.02</v>
       </c>
     </row>
@@ -3378,7 +1073,6 @@
         <v>2024</v>
       </c>
       <c r="C61" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A61,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B61,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3199999999999998</v>
       </c>
     </row>
@@ -3390,7 +1084,6 @@
         <v>2025</v>
       </c>
       <c r="C62" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A62,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B62,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2531839999999996</v>
       </c>
     </row>
@@ -3402,7 +1095,6 @@
         <v>2026</v>
       </c>
       <c r="C63" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A63,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B63,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1882923007999997</v>
       </c>
     </row>
@@ -3414,7 +1106,6 @@
         <v>2027</v>
       </c>
       <c r="C64" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A64,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B64,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1252694825369596</v>
       </c>
     </row>
@@ -3426,7 +1117,6 @@
         <v>2028</v>
       </c>
       <c r="C65" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A65,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B65,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0640617214398951</v>
       </c>
     </row>
@@ -3438,7 +1128,6 @@
         <v>2029</v>
       </c>
       <c r="C66" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A66,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B66,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0046167438624258</v>
       </c>
     </row>
@@ -3450,7 +1139,6 @@
         <v>2030</v>
       </c>
       <c r="C67" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A67,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B67,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.946883781639188</v>
       </c>
     </row>
@@ -3462,7 +1150,6 @@
         <v>2031</v>
       </c>
       <c r="C68" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A68,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B68,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9182015092274207</v>
       </c>
     </row>
@@ -3474,7 +1161,6 @@
         <v>2032</v>
       </c>
       <c r="C69" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A69,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B69,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8899417955520614</v>
       </c>
     </row>
@@ -3486,7 +1172,6 @@
         <v>2033</v>
       </c>
       <c r="C70" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A70,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B70,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8620984153083942</v>
       </c>
     </row>
@@ -3498,7 +1183,6 @@
         <v>2034</v>
       </c>
       <c r="C71" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A71,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B71,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8346652349053876</v>
       </c>
     </row>
@@ -3510,7 +1194,6 @@
         <v>2035</v>
       </c>
       <c r="C72" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A72,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B72,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8076362111145325</v>
       </c>
     </row>
@@ -3522,7 +1205,6 @@
         <v>2036</v>
       </c>
       <c r="C73" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A73,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B73,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7810053897385854</v>
       </c>
     </row>
@@ -3534,7 +1216,6 @@
         <v>2037</v>
       </c>
       <c r="C74" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A74,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B74,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.754766904299923</v>
       </c>
     </row>
@@ -3546,7 +1227,6 @@
         <v>2038</v>
       </c>
       <c r="C75" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A75,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B75,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7289149747482229</v>
       </c>
     </row>
@@ -3558,7 +1238,6 @@
         <v>2039</v>
       </c>
       <c r="C76" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A76,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B76,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7034439061871809</v>
       </c>
     </row>
@@ -3570,7 +1249,6 @@
         <v>2040</v>
       </c>
       <c r="C77" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A77,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B77,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.678348087619989</v>
       </c>
     </row>
@@ -3582,7 +1260,6 @@
         <v>2041</v>
       </c>
       <c r="C78" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A78,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B78,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6560858381247123</v>
       </c>
     </row>
@@ -3594,7 +1271,6 @@
         <v>2042</v>
       </c>
       <c r="C79" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A79,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B79,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6341188836020613</v>
       </c>
     </row>
@@ -3606,7 +1282,6 @@
         <v>2043</v>
       </c>
       <c r="C80" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A80,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B80,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6124433071468338</v>
       </c>
     </row>
@@ -3618,7 +1293,6 @@
         <v>2044</v>
       </c>
       <c r="C81" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A81,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B81,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.591055243809153</v>
       </c>
     </row>
@@ -3630,7 +1304,6 @@
         <v>2045</v>
       </c>
       <c r="C82" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A82,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B82,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.5699508799053121</v>
       </c>
     </row>
@@ -3642,7 +1315,6 @@
         <v>2046</v>
       </c>
       <c r="C83" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A83,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B83,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.5491264523377606</v>
       </c>
     </row>
@@ -3654,7 +1326,6 @@
         <v>2047</v>
       </c>
       <c r="C84" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A84,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B84,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.5285782479241095</v>
       </c>
     </row>
@@ -3666,7 +1337,6 @@
         <v>2048</v>
       </c>
       <c r="C85" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A85,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B85,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.5083026027350381</v>
       </c>
     </row>
@@ -3678,7 +1348,6 @@
         <v>2049</v>
       </c>
       <c r="C86" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A86,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B86,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.4882959014409827</v>
       </c>
     </row>
@@ -3690,7 +1359,6 @@
         <v>2050</v>
       </c>
       <c r="C87" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A87,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B87,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.4685545766674899</v>
       </c>
     </row>
@@ -3822,7 +1490,6 @@
         <v>2013</v>
       </c>
       <c r="C98" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A98,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B98,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.69</v>
       </c>
     </row>
@@ -3834,7 +1501,6 @@
         <v>2014</v>
       </c>
       <c r="C99" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A99,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B99,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.98</v>
       </c>
     </row>
@@ -3846,7 +1512,6 @@
         <v>2015</v>
       </c>
       <c r="C100" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A100,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B100,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.86</v>
       </c>
     </row>
@@ -3858,7 +1523,6 @@
         <v>2016</v>
       </c>
       <c r="C101" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A101,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B101,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.16</v>
       </c>
     </row>
@@ -3870,7 +1534,6 @@
         <v>2017</v>
       </c>
       <c r="C102" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A102,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B102,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -3882,7 +1545,6 @@
         <v>2018</v>
       </c>
       <c r="C103" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A103,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B103,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.2300000000000004</v>
       </c>
     </row>
@@ -3894,7 +1556,6 @@
         <v>2019</v>
       </c>
       <c r="C104" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A104,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B104,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.4</v>
       </c>
     </row>
@@ -3906,7 +1567,6 @@
         <v>2020</v>
       </c>
       <c r="C105" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A105,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B105,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.62</v>
       </c>
     </row>
@@ -3918,7 +1578,6 @@
         <v>2021</v>
       </c>
       <c r="C106" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A106,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B106,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.81</v>
       </c>
     </row>
@@ -3930,7 +1589,6 @@
         <v>2022</v>
       </c>
       <c r="C107" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A107,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B107,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4</v>
       </c>
     </row>
@@ -3942,7 +1600,6 @@
         <v>2023</v>
       </c>
       <c r="C108" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A108,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B108,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.03</v>
       </c>
     </row>
@@ -3954,7 +1611,6 @@
         <v>2024</v>
       </c>
       <c r="C109" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A109,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B109,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.57</v>
       </c>
     </row>
@@ -3966,7 +1622,6 @@
         <v>2025</v>
       </c>
       <c r="C110" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A110,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B110,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4959839999999995</v>
       </c>
     </row>
@@ -3978,7 +1633,6 @@
         <v>2026</v>
       </c>
       <c r="C111" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A111,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B111,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4240996607999996</v>
       </c>
     </row>
@@ -3990,7 +1644,6 @@
         <v>2027</v>
       </c>
       <c r="C112" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A112,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B112,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3542855905689595</v>
       </c>
     </row>
@@ -4002,7 +1655,6 @@
         <v>2028</v>
       </c>
       <c r="C113" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A113,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B113,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2864821655605732</v>
       </c>
     </row>
@@ -4014,7 +1666,6 @@
         <v>2029</v>
       </c>
       <c r="C114" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A114,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B114,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2206314791924284</v>
       </c>
     </row>
@@ -4026,7 +1677,6 @@
         <v>2030</v>
       </c>
       <c r="C115" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A115,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B115,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1566772925916862</v>
       </c>
     </row>
@@ -4038,7 +1688,6 @@
         <v>2031</v>
       </c>
       <c r="C116" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A116,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B116,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1249042580665818</v>
       </c>
     </row>
@@ -4050,7 +1699,6 @@
         <v>2032</v>
       </c>
       <c r="C117" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A117,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B117,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0935993166244811</v>
       </c>
     </row>
@@ -4062,7 +1710,6 @@
         <v>2033</v>
       </c>
       <c r="C118" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A118,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B118,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0627555721304187</v>
       </c>
     </row>
@@ -4074,7 +1721,6 @@
         <v>2034</v>
       </c>
       <c r="C119" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A119,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B119,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0323662300460534</v>
       </c>
     </row>
@@ -4086,7 +1732,6 @@
         <v>2035</v>
       </c>
       <c r="C120" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A120,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B120,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0024245959329079</v>
       </c>
     </row>
@@ -4098,7 +1743,6 @@
         <v>2036</v>
       </c>
       <c r="C121" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A121,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B121,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9729240739776559</v>
       </c>
     </row>
@@ -4110,7 +1754,6 @@
         <v>2037</v>
       </c>
       <c r="C122" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A122,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B122,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9438581655391376</v>
       </c>
     </row>
@@ -4122,7 +1765,6 @@
         <v>2038</v>
       </c>
       <c r="C123" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A123,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B123,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9152204677167801</v>
       </c>
     </row>
@@ -4134,7 +1776,6 @@
         <v>2039</v>
       </c>
       <c r="C124" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A124,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B124,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8870046719401088</v>
       </c>
     </row>
@@ -4146,7 +1787,6 @@
         <v>2040</v>
       </c>
       <c r="C125" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A125,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B125,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8592045625790383</v>
       </c>
     </row>
@@ -4158,7 +1798,6 @@
         <v>2041</v>
       </c>
       <c r="C126" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A126,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B126,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8345433637847017</v>
       </c>
     </row>
@@ -4170,7 +1809,6 @@
         <v>2042</v>
       </c>
       <c r="C127" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A127,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B127,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8102092805419374</v>
       </c>
     </row>
@@ -4182,7 +1820,6 @@
         <v>2043</v>
       </c>
       <c r="C128" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A128,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B128,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7861979738652414</v>
       </c>
     </row>
@@ -4194,7 +1831,6 @@
         <v>2044</v>
       </c>
       <c r="C129" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A129,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B129,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7625051623230692</v>
       </c>
     </row>
@@ -4206,7 +1842,6 @@
         <v>2045</v>
       </c>
       <c r="C130" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A130,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B130,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7391266212744181</v>
       </c>
     </row>
@@ -4218,7 +1853,6 @@
         <v>2046</v>
       </c>
       <c r="C131" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A131,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B131,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7160581821155356</v>
       </c>
     </row>
@@ -4230,7 +1864,6 @@
         <v>2047</v>
       </c>
       <c r="C132" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A132,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B132,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6932957315366204</v>
       </c>
     </row>
@@ -4242,7 +1875,6 @@
         <v>2048</v>
       </c>
       <c r="C133" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A133,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B133,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6708352107883819</v>
       </c>
     </row>
@@ -4254,7 +1886,6 @@
         <v>2049</v>
       </c>
       <c r="C134" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A134,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B134,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6486726149583291</v>
       </c>
     </row>
@@ -4266,7 +1897,6 @@
         <v>2050</v>
       </c>
       <c r="C135" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A135,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B135,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6268039922566582</v>
       </c>
     </row>
@@ -4398,7 +2028,6 @@
         <v>2013</v>
       </c>
       <c r="C146" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A146,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B146,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.8203246753246765</v>
       </c>
     </row>
@@ -4410,7 +2039,6 @@
         <v>2014</v>
       </c>
       <c r="C147" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A147,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B147,[1]calculos!$B$11:$AM$11,0))</f>
         <v>7.115974025974027</v>
       </c>
     </row>
@@ -4422,7 +2050,6 @@
         <v>2015</v>
       </c>
       <c r="C148" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A148,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B148,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.993636363636365</v>
       </c>
     </row>
@@ -4434,7 +2061,6 @@
         <v>2016</v>
       </c>
       <c r="C149" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A149,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B149,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.28</v>
       </c>
     </row>
@@ -4446,7 +2072,6 @@
         <v>2017</v>
       </c>
       <c r="C150" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A150,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B150,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.47</v>
       </c>
     </row>
@@ -4458,7 +2083,6 @@
         <v>2018</v>
       </c>
       <c r="C151" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A151,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B151,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.2300000000000004</v>
       </c>
     </row>
@@ -4470,7 +2094,6 @@
         <v>2019</v>
       </c>
       <c r="C152" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A152,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B152,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.5</v>
       </c>
     </row>
@@ -4482,7 +2105,6 @@
         <v>2020</v>
       </c>
       <c r="C153" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A153,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B153,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.85</v>
       </c>
     </row>
@@ -4494,7 +2116,6 @@
         <v>2021</v>
       </c>
       <c r="C154" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A154,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B154,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.08</v>
       </c>
     </row>
@@ -4506,7 +2127,6 @@
         <v>2022</v>
       </c>
       <c r="C155" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A155,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B155,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.45</v>
       </c>
     </row>
@@ -4518,7 +2138,6 @@
         <v>2023</v>
       </c>
       <c r="C156" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A156,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B156,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.64</v>
       </c>
     </row>
@@ -4530,7 +2149,6 @@
         <v>2024</v>
       </c>
       <c r="C157" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A157,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B157,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.13</v>
       </c>
     </row>
@@ -4542,7 +2160,6 @@
         <v>2025</v>
       </c>
       <c r="C158" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A158,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B158,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.0398559999999999</v>
       </c>
     </row>
@@ -4554,7 +2171,6 @@
         <v>2026</v>
       </c>
       <c r="C159" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A159,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B159,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.9523081471999997</v>
       </c>
     </row>
@@ -4566,7 +2182,6 @@
         <v>2027</v>
       </c>
       <c r="C160" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A160,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B160,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.8672816725606394</v>
       </c>
     </row>
@@ -4578,7 +2193,6 @@
         <v>2028</v>
       </c>
       <c r="C161" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A161,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B161,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.784703960390893</v>
       </c>
     </row>
@@ -4590,7 +2204,6 @@
         <v>2029</v>
       </c>
       <c r="C162" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A162,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B162,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.704504486331635</v>
       </c>
     </row>
@@ -4602,7 +2215,6 @@
         <v>2030</v>
       </c>
       <c r="C163" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A163,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B163,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.6266147571252838</v>
       </c>
     </row>
@@ -4614,7 +2226,6 @@
         <v>2031</v>
       </c>
       <c r="C164" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A164,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B164,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.5879184154663046</v>
       </c>
     </row>
@@ -4626,7 +2237,6 @@
         <v>2032</v>
       </c>
       <c r="C165" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A165,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B165,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.5497921638267038</v>
       </c>
     </row>
@@ -4638,7 +2248,6 @@
         <v>2033</v>
       </c>
       <c r="C166" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A166,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B166,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.5122276034117563</v>
       </c>
     </row>
@@ -4650,7 +2259,6 @@
         <v>2034</v>
       </c>
       <c r="C167" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A167,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B167,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4752164591611483</v>
       </c>
     </row>
@@ -4662,7 +2270,6 @@
         <v>2035</v>
       </c>
       <c r="C168" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A168,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B168,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4387505779260725</v>
       </c>
     </row>
@@ -4674,7 +2281,6 @@
         <v>2036</v>
       </c>
       <c r="C169" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A169,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B169,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4028219266731781</v>
       </c>
     </row>
@@ -4686,7 +2292,6 @@
         <v>2037</v>
       </c>
       <c r="C170" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A170,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B170,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3674225907149826</v>
       </c>
     </row>
@@ -4698,7 +2303,6 @@
         <v>2038</v>
       </c>
       <c r="C171" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A171,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B171,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3325447719663526</v>
       </c>
     </row>
@@ -4710,7 +2314,6 @@
         <v>2039</v>
       </c>
       <c r="C172" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A172,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B172,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2981807872266709</v>
       </c>
     </row>
@@ -4722,7 +2325,6 @@
         <v>2040</v>
       </c>
       <c r="C173" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A173,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B173,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2643230664873126</v>
       </c>
     </row>
@@ -4734,7 +2336,6 @@
         <v>2041</v>
       </c>
       <c r="C174" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A174,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B174,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2342882212630819</v>
       </c>
     </row>
@@ -4746,7 +2347,6 @@
         <v>2042</v>
       </c>
       <c r="C175" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A175,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B175,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2046517696872638</v>
       </c>
     </row>
@@ -4758,7 +2358,6 @@
         <v>2043</v>
       </c>
       <c r="C176" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A176,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B176,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1754084273144785</v>
       </c>
     </row>
@@ -4770,7 +2369,6 @@
         <v>2044</v>
       </c>
       <c r="C177" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A177,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B177,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1465529797942455</v>
       </c>
     </row>
@@ -4782,7 +2380,6 @@
         <v>2045</v>
       </c>
       <c r="C178" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A178,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B178,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1180802819412188</v>
       </c>
     </row>
@@ -4794,7 +2391,6 @@
         <v>2046</v>
       </c>
       <c r="C179" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A179,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B179,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.089985256817755</v>
       </c>
     </row>
@@ -4806,7 +2402,6 @@
         <v>2047</v>
       </c>
       <c r="C180" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A180,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B180,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0622628948286481</v>
       </c>
     </row>
@@ -4818,7 +2413,6 @@
         <v>2048</v>
       </c>
       <c r="C181" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A181,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B181,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0349082528278752</v>
       </c>
     </row>
@@ -4830,7 +2424,6 @@
         <v>2049</v>
       </c>
       <c r="C182" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A182,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B182,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0079164532371885</v>
       </c>
     </row>
@@ -4842,7 +2435,6 @@
         <v>2050</v>
       </c>
       <c r="C183" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A183,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B183,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9812826831763986</v>
       </c>
     </row>
@@ -4974,7 +2566,6 @@
         <v>2013</v>
       </c>
       <c r="C194" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A194,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B194,[1]calculos!$B$11:$AM$11,0))</f>
         <v>7.7303680981595102</v>
       </c>
     </row>
@@ -4986,7 +2577,6 @@
         <v>2014</v>
       </c>
       <c r="C195" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A195,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B195,[1]calculos!$B$11:$AM$11,0))</f>
         <v>7.8371165644171796</v>
       </c>
     </row>
@@ -4998,7 +2588,6 @@
         <v>2015</v>
       </c>
       <c r="C196" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A196,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B196,[1]calculos!$B$11:$AM$11,0))</f>
         <v>7.6325153374233139</v>
       </c>
     </row>
@@ -5010,7 +2599,6 @@
         <v>2016</v>
       </c>
       <c r="C197" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A197,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B197,[1]calculos!$B$11:$AM$11,0))</f>
         <v>6.6806748466257675</v>
       </c>
     </row>
@@ -5022,7 +2610,6 @@
         <v>2017</v>
       </c>
       <c r="C198" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A198,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B198,[1]calculos!$B$11:$AM$11,0))</f>
         <v>5.8</v>
       </c>
     </row>
@@ -5034,7 +2621,6 @@
         <v>2018</v>
       </c>
       <c r="C199" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A199,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B199,[1]calculos!$B$11:$AM$11,0))</f>
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -5046,7 +2632,6 @@
         <v>2019</v>
       </c>
       <c r="C200" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A200,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B200,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -5058,7 +2643,6 @@
         <v>2020</v>
       </c>
       <c r="C201" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A201,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B201,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.2699999999999996</v>
       </c>
     </row>
@@ -5070,7 +2654,6 @@
         <v>2021</v>
       </c>
       <c r="C202" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A202,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B202,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.38</v>
       </c>
       <c r="E202" s="1"/>
@@ -5083,7 +2666,6 @@
         <v>2022</v>
       </c>
       <c r="C203" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A203,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B203,[1]calculos!$B$11:$AM$11,0))</f>
         <v>4.3499999999999996</v>
       </c>
       <c r="E203" s="1"/>
@@ -5096,7 +2678,6 @@
         <v>2023</v>
       </c>
       <c r="C204" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A204,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B204,[1]calculos!$B$11:$AM$11,0))</f>
         <v>3.26</v>
       </c>
       <c r="E204" s="1"/>
@@ -5109,7 +2690,6 @@
         <v>2024</v>
       </c>
       <c r="C205" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A205,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B205,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.58</v>
       </c>
       <c r="E205" s="1"/>
@@ -5122,7 +2702,6 @@
         <v>2025</v>
       </c>
       <c r="C206" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A206,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B206,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.5056959999999999</v>
       </c>
       <c r="E206" s="1"/>
@@ -5135,7 +2714,6 @@
         <v>2026</v>
       </c>
       <c r="C207" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A207,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B207,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.4335319551999999</v>
       </c>
       <c r="E207" s="1"/>
@@ -5148,7 +2726,6 @@
         <v>2027</v>
       </c>
       <c r="C208" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A208,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B208,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.3634462348902399</v>
       </c>
       <c r="E208" s="1"/>
@@ -5161,7 +2738,6 @@
         <v>2028</v>
       </c>
       <c r="C209" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A209,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B209,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.295378983325401</v>
       </c>
       <c r="E209" s="1"/>
@@ -5174,7 +2750,6 @@
         <v>2029</v>
       </c>
       <c r="C210" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A210,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B210,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.2292720686056295</v>
       </c>
       <c r="E210" s="1"/>
@@ -5187,7 +2762,6 @@
         <v>2030</v>
       </c>
       <c r="C211" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A211,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B211,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1650690330297873</v>
       </c>
       <c r="E211" s="1"/>
@@ -5200,7 +2774,6 @@
         <v>2031</v>
       </c>
       <c r="C212" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A212,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B212,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1331723680201495</v>
       </c>
       <c r="E212" s="1"/>
@@ -5213,7 +2786,6 @@
         <v>2032</v>
       </c>
       <c r="C213" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A213,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B213,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.1017456174673792</v>
       </c>
       <c r="E213" s="1"/>
@@ -5226,7 +2798,6 @@
         <v>2033</v>
       </c>
       <c r="C214" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A214,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B214,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0707818584033011</v>
       </c>
       <c r="E214" s="1"/>
@@ -5239,7 +2810,6 @@
         <v>2034</v>
       </c>
       <c r="C215" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A215,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B215,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0402742698516816</v>
       </c>
       <c r="E215" s="1"/>
@@ -5252,7 +2822,6 @@
         <v>2035</v>
       </c>
       <c r="C216" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A216,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B216,[1]calculos!$B$11:$AM$11,0))</f>
         <v>2.0102161313256444</v>
       </c>
       <c r="E216" s="1"/>
@@ -5265,7 +2834,6 @@
         <v>2036</v>
       </c>
       <c r="C217" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A217,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B217,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9806008213472202</v>
       </c>
       <c r="E217" s="1"/>
@@ -5278,7 +2846,6 @@
         <v>2037</v>
       </c>
       <c r="C218" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A218,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B218,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9514218159887076</v>
       </c>
       <c r="E218" s="1"/>
@@ -5291,7 +2858,6 @@
         <v>2038</v>
       </c>
       <c r="C219" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A219,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B219,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.9226726874355238</v>
       </c>
       <c r="E219" s="1"/>
@@ -5304,7 +2870,6 @@
         <v>2039</v>
       </c>
       <c r="C220" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A220,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B220,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8943471025702272</v>
       </c>
       <c r="E220" s="1"/>
@@ -5317,7 +2882,6 @@
         <v>2040</v>
       </c>
       <c r="C221" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A221,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B221,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8664388215774017</v>
       </c>
       <c r="E221" s="1"/>
@@ -5330,7 +2894,6 @@
         <v>2041</v>
       </c>
       <c r="C222" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A222,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B222,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.8416816648111027</v>
       </c>
       <c r="E222" s="1"/>
@@ -5343,7 +2906,6 @@
         <v>2042</v>
       </c>
       <c r="C223" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A223,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B223,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.817252896419534</v>
       </c>
       <c r="E223" s="1"/>
@@ -5356,7 +2918,6 @@
         <v>2043</v>
       </c>
       <c r="C224" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A224,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B224,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7931481605339794</v>
       </c>
       <c r="E224" s="1"/>
@@ -5369,7 +2930,6 @@
         <v>2044</v>
       </c>
       <c r="C225" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A225,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B225,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7693631590636276</v>
       </c>
       <c r="E225" s="1"/>
@@ -5382,7 +2942,6 @@
         <v>2045</v>
       </c>
       <c r="C226" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A226,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B226,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.745893650929184</v>
       </c>
       <c r="E226" s="1"/>
@@ -5395,7 +2954,6 @@
         <v>2046</v>
       </c>
       <c r="C227" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A227,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B227,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.7227354513066484</v>
       </c>
       <c r="E227" s="1"/>
@@ -5408,7 +2966,6 @@
         <v>2047</v>
       </c>
       <c r="C228" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A228,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B228,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6998844308811227</v>
       </c>
       <c r="E228" s="1"/>
@@ -5421,7 +2978,6 @@
         <v>2048</v>
       </c>
       <c r="C229" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A229,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B229,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6773365151105175</v>
       </c>
       <c r="E229" s="1"/>
@@ -5434,7 +2990,6 @@
         <v>2049</v>
       </c>
       <c r="C230" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A230,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B230,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6550876834990247</v>
       </c>
       <c r="E230" s="1"/>
@@ -5447,7 +3002,6 @@
         <v>2050</v>
       </c>
       <c r="C231" s="1">
-        <f>INDEX([1]calculos!$B$12:$AM$16,MATCH([1]custos!A231,[1]calculos!$A$12:$A$16,0),MATCH([1]custos!B231,[1]calculos!$B$11:$AM$11,0))</f>
         <v>1.6331339688802267</v>
       </c>
       <c r="E231" s="1"/>

</xml_diff>